<commit_message>
kpi pagination, show user name kpi, alicia maju bisa edit kpi sendiri
</commit_message>
<xml_diff>
--- a/public/import/DAILY ADITYO.xlsx
+++ b/public/import/DAILY ADITYO.xlsx
@@ -83,22 +83,22 @@
     <t>SERAH TERIMA BARANG DATANG DAN KELUAR</t>
   </si>
   <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-20</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
-    <t>2023-09-23</t>
+    <t>2023-09-25</t>
+  </si>
+  <si>
+    <t>2023-09-26</t>
+  </si>
+  <si>
+    <t>2023-09-27</t>
+  </si>
+  <si>
+    <t>2023-09-28</t>
+  </si>
+  <si>
+    <t>2023-09-29</t>
+  </si>
+  <si>
+    <t>2023-09-30</t>
   </si>
 </sst>
 </file>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>